<commit_message>
Modificacion del libro del excel
</commit_message>
<xml_diff>
--- a/PEsperanza.xlsx
+++ b/PEsperanza.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="LISTADO PERSONAL ESPERANZA" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="23">
-  <si>
-    <t xml:space="preserve">PERSONAL LA ESPERANZA</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="22">
   <si>
     <t xml:space="preserve">N°</t>
   </si>
@@ -98,7 +95,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -123,7 +120,7 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="8"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -131,21 +128,6 @@
     </font>
     <font>
       <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -166,19 +148,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium"/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -214,7 +189,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -227,24 +202,16 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -508,10 +475,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.71484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -520,217 +487,207 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="18.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="29.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="27.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16374" style="0" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16374" style="2" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="5"/>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="6" t="s">
+      <c r="B2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>7</v>
+      <c r="B3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>8</v>
+      <c r="A4" s="7" t="n">
+        <v>4</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>7</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="9" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="9" t="s">
+      <c r="A5" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="7" t="n">
         <v>8</v>
       </c>
-      <c r="D5" s="10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="n">
-        <v>7</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>8</v>
+      <c r="B6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>7</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="9" t="n">
-        <v>8</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="10" t="s">
+      <c r="A7" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="n">
-        <v>9</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>8</v>
+      <c r="A8" s="7" t="n">
+        <v>10</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="9" t="n">
-        <v>10</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="10" t="s">
+      <c r="A9" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="D9" s="6" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4" t="n">
-        <v>11</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>16</v>
+      <c r="A10" s="7" t="n">
+        <v>12</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>15</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="9" t="n">
-        <v>12</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="9" t="s">
+      <c r="A11" s="5" t="n">
+        <v>13</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="5" t="n">
+        <v>14</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="7" t="n">
+        <v>15</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="5" t="n">
         <v>16</v>
       </c>
-      <c r="D11" s="10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4" t="n">
-        <v>13</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4" t="n">
-        <v>14</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="9" t="n">
-        <v>15</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" s="8" t="s">
+      <c r="B14" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="4" t="n">
-        <v>16</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>22</v>
-      </c>
-    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:B1"/>
-  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>